<commit_message>
modified all figures, and numbers in text
</commit_message>
<xml_diff>
--- a/Data/Simulation Data/ComparingPV_Data.xlsx
+++ b/Data/Simulation Data/ComparingPV_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="640" windowWidth="27680" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="3420" yWindow="3100" windowWidth="21400" windowHeight="11740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Embodied</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ASF CH incl shading</t>
   </si>
   <si>
-    <t>ASF ENTSO-E excl shading benefits</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -118,7 +115,19 @@
     <t>Orientated solar façade ENTSO-E excl shading</t>
   </si>
   <si>
-    <t>Orientated solar facade ASF ENTSO-E incl shading</t>
+    <t>Orientated solar facade ASF german incl shading</t>
+  </si>
+  <si>
+    <t>ASF german excl shading benefits</t>
+  </si>
+  <si>
+    <t>ASF german incl shading</t>
+  </si>
+  <si>
+    <t>ASF german incl shading motorized</t>
+  </si>
+  <si>
+    <t>ASF Madrid</t>
   </si>
 </sst>
 </file>
@@ -128,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,8 +191,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +214,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -240,7 +261,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -250,8 +271,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -264,14 +298,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="9" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="9" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -549,126 +597,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>2675.4</v>
+        <v>2498</v>
       </c>
       <c r="C2" s="1">
-        <v>2675.4</v>
+        <v>2498</v>
       </c>
       <c r="D2" s="1">
-        <v>2675.4</v>
+        <v>2498</v>
       </c>
       <c r="E2" s="1">
-        <v>2675.4</v>
+        <v>2498</v>
       </c>
       <c r="F2" s="1">
-        <v>3251.2</v>
+        <v>2498</v>
       </c>
       <c r="G2" s="1">
-        <v>3251.2</v>
+        <f>$F$2+575.6</f>
+        <v>3073.6</v>
       </c>
       <c r="H2" s="1">
-        <v>2692</v>
+        <f>$F$2+575.6</f>
+        <v>3073.6</v>
       </c>
       <c r="I2" s="1">
-        <v>2352.3000000000002</v>
+        <f>D2+17</f>
+        <v>2515</v>
       </c>
       <c r="J2" s="1">
-        <v>2352.3000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <f>$F$2-323.1</f>
+        <v>2174.9</v>
+      </c>
+      <c r="K2" s="1">
+        <f>$F$2-323.1</f>
+        <v>2174.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f>-1021.8*20*0.4621</f>
-        <v>-9443.4755999999998</v>
+        <f>-929*20*0.6109</f>
+        <v>-11350.522000000001</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
+        <f>-1658*20*0.4489</f>
+        <v>-14885.524000000001</v>
+      </c>
+      <c r="E3" s="1">
         <f>-1021.8*20*0.1131</f>
         <v>-2311.3116</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <f>-1021.8*20*0.6109</f>
         <v>-12484.3524</v>
       </c>
-      <c r="F3" s="1">
-        <f>-1021.8*20*0.4621</f>
-        <v>-9443.4755999999998</v>
-      </c>
       <c r="G3" s="1">
+        <f>-929*20*0.6109</f>
+        <v>-11350.522000000001</v>
+      </c>
+      <c r="H3" s="1">
         <f>-1021.8*20*0.1131</f>
         <v>-2311.3116</v>
       </c>
-      <c r="H3" s="1">
-        <f>-1021.8*20*0.4621</f>
-        <v>-9443.4755999999998</v>
-      </c>
       <c r="I3" s="1">
-        <f>-780*20*0.4621</f>
-        <v>-7208.76</v>
+        <f>-929*20*0.6109</f>
+        <v>-11350.522000000001</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <f>-712*20*0.6109</f>
+        <v>-8699.2160000000003</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -681,33 +744,37 @@
         <v>225.87817680000001</v>
       </c>
       <c r="D4" s="1">
+        <f>0.31/1000*4*54*365*20*0.4621</f>
+        <v>225.87817680000001</v>
+      </c>
+      <c r="E4" s="1">
         <f>0.31/1000*4*54*365*20*0.1131</f>
         <v>55.284184800000006</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <f>0.31/1000*4*54*365*20*0.6109</f>
         <v>298.61280720000002</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <f>15.8*0.4621</f>
         <v>7.3011800000000004</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f>15.8*0.1131</f>
         <v>1.7869800000000002</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <f>0.31/1000*4*54*365*20*0.4621</f>
         <v>225.87817680000001</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -728,23 +795,27 @@
         <v>235.61999999999998</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
         <f>(42.73+35.81)*3</f>
         <v>235.61999999999998</v>
       </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <f>(42.73+35.81)*3</f>
+        <v>235.61999999999998</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -755,89 +826,96 @@
         <v>77</v>
       </c>
       <c r="D6" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1">
         <v>77</v>
       </c>
       <c r="F6" s="1">
-        <v>86.5</v>
+        <v>77</v>
       </c>
       <c r="G6" s="1">
         <v>86.5</v>
       </c>
       <c r="H6" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="I6" s="1">
         <v>77</v>
-      </c>
-      <c r="I6" s="1">
-        <v>74.099999999999994</v>
       </c>
       <c r="J6" s="1">
         <v>74.099999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="1">
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <f>SUM(B2:B6)</f>
-        <v>-6229.5774232000003</v>
+        <v>-8314.0238231999992</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" ref="C7:D7" si="0">SUM(C2:C6)</f>
-        <v>3213.8981767999999</v>
+        <f>SUM(C2:C6)</f>
+        <v>3036.4981767999998</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>731.99258480000003</v>
+        <f>SUM(D2:D6)</f>
+        <v>-11848.0258232</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7" si="1">SUM(E2:E6)</f>
-        <v>-9197.7195928000001</v>
+        <f t="shared" ref="E7" si="0">SUM(E2:E6)</f>
+        <v>554.59258479999994</v>
       </c>
       <c r="F7" s="3">
-        <f>SUM(F2:F6)</f>
-        <v>-6098.4744199999996</v>
+        <f t="shared" ref="F7" si="1">SUM(F2:F6)</f>
+        <v>-9375.1195927999997</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>1028.1753799999997</v>
+        <v>-8183.1208200000001</v>
       </c>
       <c r="H7" s="3">
         <f>SUM(H2:H6)</f>
-        <v>-6212.9774232</v>
+        <v>850.57537999999988</v>
       </c>
       <c r="I7" s="3">
         <f>SUM(I2:I6)</f>
-        <v>-4782.3599999999997</v>
+        <v>-8297.0238231999992</v>
       </c>
       <c r="J7" s="3">
         <f>SUM(J2:J6)</f>
-        <v>2426.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>-6450.2160000000003</v>
+      </c>
+      <c r="K7" s="3">
+        <f>SUM(K2:K6)</f>
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11">
-        <f t="shared" ref="B9:H9" si="2">518.1946*20</f>
-        <v>10363.892</v>
+        <f>458.7*20</f>
+        <v>9174</v>
       </c>
       <c r="C9" s="11">
-        <f t="shared" si="2"/>
-        <v>10363.892</v>
+        <f>458.7*20</f>
+        <v>9174</v>
       </c>
       <c r="D9" s="11">
-        <f t="shared" si="2"/>
-        <v>10363.892</v>
+        <f>718*20</f>
+        <v>14360</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E9:I9" si="2">518.1946*20</f>
         <v>10363.892</v>
       </c>
       <c r="F9" s="11">
@@ -845,94 +923,103 @@
         <v>10363.892</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="2"/>
-        <v>10363.892</v>
+        <f>458.7*20</f>
+        <v>9174</v>
       </c>
       <c r="H9" s="11">
         <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="I9" s="11">
-        <f>471.086*20</f>
-        <v>9421.7200000000012</v>
+        <f>458.7*20</f>
+        <v>9174</v>
       </c>
       <c r="J9" s="11">
-        <f>471.086*20</f>
-        <v>9421.7200000000012</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <f>417*20</f>
+        <v>8340</v>
+      </c>
+      <c r="K9" s="11">
+        <f>417*20</f>
+        <v>8340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
         <f>B7/B9*1000</f>
-        <v>-601.08474916566104</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" ref="C11:D11" si="3">C7/C9*1000</f>
-        <v>310.10533270705639</v>
-      </c>
-      <c r="D11" s="3">
+        <v>-906.25940954872453</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" ref="C11:E11" si="3">C7/C9*1000</f>
+        <v>330.98955491606711</v>
+      </c>
+      <c r="D11" s="12">
         <f t="shared" si="3"/>
-        <v>70.629121260622938</v>
+        <v>-825.07143615598886</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ref="E11" si="4">E7/E9*1000</f>
-        <v>-887.47736784597907</v>
+        <f t="shared" si="3"/>
+        <v>53.511999623307538</v>
       </c>
       <c r="F11" s="3">
-        <f>F7/F9*1000</f>
-        <v>-588.43477141598919</v>
+        <f t="shared" ref="F11" si="4">F7/F9*1000</f>
+        <v>-904.59448948329441</v>
       </c>
       <c r="G11" s="3">
         <f>G7/G9*1000</f>
-        <v>99.207457970422666</v>
+        <v>-891.99049705689993</v>
       </c>
       <c r="H11" s="3">
         <f>H7/H9*1000</f>
-        <v>-599.48303428866302</v>
+        <v>82.071038563504899</v>
       </c>
       <c r="I11" s="3">
         <f>I7/I9*1000</f>
-        <v>-507.58884789613779</v>
-      </c>
-      <c r="J11" s="3">
+        <v>-904.40634654458245</v>
+      </c>
+      <c r="J11" s="12">
         <f>J7/J9*1000</f>
-        <v>257.53259489774689</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>-773.4071942446044</v>
+      </c>
+      <c r="K11" s="12">
+        <f>K7/K9*1000</f>
+        <v>269.66426858513188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="B15" s="1">
+        <v>855</v>
+      </c>
+      <c r="C15" s="1">
+        <v>855</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" s="1">
-        <v>966</v>
-      </c>
-      <c r="C15" s="1">
-        <v>966</v>
-      </c>
-      <c r="D15">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>21</v>
       </c>
       <c r="B16" s="7">
         <v>0.6944444444444442</v>
@@ -940,13 +1027,14 @@
       <c r="C16" s="7">
         <v>0.6944444444444442</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
         <v>0.6944444444444442</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7">
         <v>0.38470000000000004</v>
@@ -954,27 +1042,29 @@
       <c r="C17" s="7">
         <v>0.38470000000000004</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7"/>
+      <c r="E17">
         <v>0.38470000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>365.33437499999985</v>
+      </c>
+      <c r="C18" s="1">
+        <v>365.33437499999985</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18">
+        <v>365.33437499999985</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>23</v>
-      </c>
-      <c r="B18" s="1">
-        <v>412.76374999999979</v>
-      </c>
-      <c r="C18" s="1">
-        <v>412.76374999999979</v>
-      </c>
-      <c r="D18">
-        <v>412.76374999999979</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>24</v>
       </c>
       <c r="B19" s="7">
         <v>0.14000000000000001</v>
@@ -982,28 +1072,30 @@
       <c r="C19" s="7">
         <v>0.11</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7"/>
+      <c r="E19">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
         <v>25</v>
-      </c>
-      <c r="B20" s="7">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>26</v>
       </c>
       <c r="B21" s="7">
         <v>1</v>
@@ -1011,28 +1103,30 @@
       <c r="C21" s="7">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7"/>
+      <c r="E21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
-        <v>878.36125999999956</v>
+        <v>777.43154999999967</v>
       </c>
       <c r="C22" s="10">
-        <v>690.14098999999965</v>
-      </c>
-      <c r="D22" s="10">
-        <v>627.40089999999964</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>610.83907499999964</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10">
+        <v>555.3082499999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1042,11 +1136,11 @@
       <c r="C24">
         <v>2020.8</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1600.97</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1056,11 +1150,11 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1070,11 +1164,11 @@
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1084,11 +1178,11 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1098,42 +1192,44 @@
       <c r="C28">
         <v>3.09</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>3.09</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2">
         <f>SUM(B24:B28)</f>
         <v>3037.1580000000004</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" ref="C29:D29" si="5">SUM(C24:C28)</f>
+        <f t="shared" ref="C29:E29" si="5">SUM(C24:C28)</f>
         <v>2023.8899999999999</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
         <f t="shared" si="5"/>
         <v>1604.06</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="3">
+        <v>9</v>
+      </c>
+      <c r="B31" s="12">
         <f>B29/(B22*20)*1000</f>
-        <v>172.88774780436026</v>
-      </c>
-      <c r="C31" s="3">
+        <v>195.33282383510172</v>
+      </c>
+      <c r="C31" s="12">
         <f>C29/(C22*20)*1000</f>
-        <v>146.62873451408825</v>
-      </c>
-      <c r="D31" s="3">
-        <f>D29/(D22*20)*1000</f>
-        <v>127.83373437940566</v>
+        <v>165.6647456615313</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12">
+        <f>E29/(E22*20)*1000</f>
+        <v>144.42969287778462</v>
       </c>
     </row>
   </sheetData>
@@ -1169,7 +1265,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1177,7 +1273,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1267,7 +1363,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <f>SUM(B3:B7)</f>
@@ -1288,7 +1384,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" ref="B10:F10" si="0">580*20</f>
@@ -1306,7 +1402,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <f>B8/B10*1000</f>
@@ -1324,7 +1420,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <f>0.31/1000*$B$18*54*365*20*0.4621</f>
@@ -1340,7 +1436,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5">
         <v>6</v>
@@ -1348,7 +1444,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6">
         <f>F12-B12</f>

</xml_diff>